<commit_message>
Updated the following workbook with new test data - VerifyReq_UpdateQuantityAndSaveCart.
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyReq_UpdateQuantityAndSaveCart.xlsx
+++ b/src/test/resources/datasheets/VerifyReq_UpdateQuantityAndSaveCart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="330" windowWidth="14220" windowHeight="2445"/>
   </bookViews>
   <sheets>
     <sheet name="UpdateQuantityAndSaveCart" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Role</t>
   </si>
@@ -28,6 +29,9 @@
   </si>
   <si>
     <t>XEEVA -MJ</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -359,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -371,19 +375,25 @@
     <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Developed a new test in catalog module - VerifyReq_UpdateQuantityAndSaveCart(). 2. Added a new method in CartInformationPage - verify_UpdatedQuantity().
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/VerifyReq_UpdateQuantityAndSaveCart.xlsx
+++ b/src/test/resources/datasheets/VerifyReq_UpdateQuantityAndSaveCart.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Role</t>
   </si>
@@ -32,6 +31,9 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -67,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,7 +369,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -393,8 +396,8 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>3</v>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>